<commit_message>
Adapting new template for mobile devices
</commit_message>
<xml_diff>
--- a/data/promo/pr.xlsx
+++ b/data/promo/pr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Service</t>
   </si>
@@ -56,6 +56,21 @@
   </si>
   <si>
     <t>$23.99</t>
+  </si>
+  <si>
+    <t>Women's Haircut and Blowout</t>
+  </si>
+  <si>
+    <t>$49.99</t>
+  </si>
+  <si>
+    <t>$34.99</t>
+  </si>
+  <si>
+    <t>Gel Manicure</t>
+  </si>
+  <si>
+    <t>$29.99</t>
   </si>
 </sst>
 </file>
@@ -388,16 +403,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -454,6 +469,28 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>